<commit_message>
update target editor tooltip
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:NO10"/>
+  <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
@@ -690,7 +689,6 @@
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>LU18</t>

</xml_diff>